<commit_message>
Data table example is added
</commit_message>
<xml_diff>
--- a/src/test/resources/users.xlsx
+++ b/src/test/resources/users.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lakshaman\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{81FC16E3-5D1C-4637-937B-FA3111313446}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{96A7BC5E-B378-49DD-ACC2-8F2FD94A7F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F911DB2-A0F2-4697-997F-07699C3077F6}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20760" windowHeight="11820" xr2:uid="{8F911DB2-A0F2-4697-997F-07699C3077F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
   <si>
     <t>FULL NAME</t>
   </si>
@@ -63,16 +59,82 @@
     <t>Kalyan K</t>
   </si>
   <si>
-    <t>manoj.pvn@heraizen.com</t>
-  </si>
-  <si>
-    <t>rajesh.t@heraizen.com</t>
-  </si>
-  <si>
-    <t>kalyan.k@heraizen.com</t>
-  </si>
-  <si>
     <t>user@$$34</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>Jayesh</t>
+  </si>
+  <si>
+    <t>Jayesh J</t>
+  </si>
+  <si>
+    <t>Suresh S</t>
+  </si>
+  <si>
+    <t>Ramesh R</t>
+  </si>
+  <si>
+    <t>Bhoomika B</t>
+  </si>
+  <si>
+    <t>Sri Lakshmi</t>
+  </si>
+  <si>
+    <t>Anusha</t>
+  </si>
+  <si>
+    <t>Abhi S</t>
+  </si>
+  <si>
+    <t>Abhi</t>
+  </si>
+  <si>
+    <t>Anusha A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sai </t>
+  </si>
+  <si>
+    <t>Sai S</t>
+  </si>
+  <si>
+    <t>Lakshmi A</t>
+  </si>
+  <si>
+    <t>Sri</t>
+  </si>
+  <si>
+    <t>manoj@heraizen.com</t>
+  </si>
+  <si>
+    <t>rajesh@heraizen.com</t>
+  </si>
+  <si>
+    <t>kalyan@heraizen.com</t>
+  </si>
+  <si>
+    <t>suresh@heraizen.com</t>
+  </si>
+  <si>
+    <t>jayesh@heraizen.com</t>
+  </si>
+  <si>
+    <t>sri@heraizen.com</t>
+  </si>
+  <si>
+    <t>lakshmi a@heraizen.com</t>
+  </si>
+  <si>
+    <t>sai @heraizen.com</t>
+  </si>
+  <si>
+    <t>anusha@heraizen.com</t>
+  </si>
+  <si>
+    <t>abhi@heraizen.com</t>
   </si>
 </sst>
 </file>
@@ -441,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3A02DE4-7F99-4659-8589-CCD84C27463D}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,9 +515,10 @@
     <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="38" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -469,7 +532,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -477,13 +540,13 @@
         <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -491,13 +554,13 @@
         <v>5</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -505,21 +568,165 @@
         <v>6</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>13</v>
+      <c r="C6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{1EF0999D-1779-4247-A3D8-17DF24B8E04A}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{99110792-1A15-441E-BF8D-D1F3387AD3C8}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{6F7BCD2C-E60B-450F-8EAE-9FF1A6AFC194}"/>
+    <hyperlink ref="C2" r:id="rId1" display="manoj.pvn@heraizen.com" xr:uid="{1EF0999D-1779-4247-A3D8-17DF24B8E04A}"/>
+    <hyperlink ref="C3" r:id="rId2" display="rajesh.t@heraizen.com" xr:uid="{99110792-1A15-441E-BF8D-D1F3387AD3C8}"/>
+    <hyperlink ref="C4" r:id="rId3" display="kalyan.k@heraizen.com" xr:uid="{6F7BCD2C-E60B-450F-8EAE-9FF1A6AFC194}"/>
     <hyperlink ref="D2" r:id="rId4" xr:uid="{FA59EBBA-825F-49D7-B78B-93EC60C9323B}"/>
     <hyperlink ref="D3" r:id="rId5" xr:uid="{655F040E-0AB8-44E4-A753-014FF2137FD1}"/>
     <hyperlink ref="D4" r:id="rId6" xr:uid="{191CA5AD-2437-4B06-B0C4-B323CE02FFBE}"/>
+    <hyperlink ref="C5" r:id="rId7" display="manoj.pvn@heraizen.com" xr:uid="{FEBBE4BF-6D5A-494E-A743-47E872C40EBB}"/>
+    <hyperlink ref="C6" r:id="rId8" display="rajesh.t@heraizen.com" xr:uid="{69FE9D39-FA06-48E4-A8E2-421972D6D30B}"/>
+    <hyperlink ref="C7" r:id="rId9" display="kalyan.k@heraizen.com" xr:uid="{6DEA021D-7854-4CC8-B349-C19D7FE35812}"/>
+    <hyperlink ref="D5" r:id="rId10" xr:uid="{1A7CB11E-608B-40D9-921E-13F8F4E554AD}"/>
+    <hyperlink ref="D6" r:id="rId11" xr:uid="{9DBE1F47-7BF1-4D73-B91A-8E999AD356EC}"/>
+    <hyperlink ref="D7" r:id="rId12" xr:uid="{7C39061F-98A5-4C2C-BA25-0B68FF83E0A3}"/>
+    <hyperlink ref="C8" r:id="rId13" display="manoj.pvn@heraizen.com" xr:uid="{0E68F52E-CC30-4E26-851D-4D6BD8F3CE4F}"/>
+    <hyperlink ref="C9" r:id="rId14" display="rajesh.t@heraizen.com" xr:uid="{3F511A16-3C4F-451D-834D-0C55A0CDD23C}"/>
+    <hyperlink ref="C10" r:id="rId15" display="kalyan.k@heraizen.com" xr:uid="{4D4D107B-2F31-412E-B7C8-069E001EB80C}"/>
+    <hyperlink ref="D8" r:id="rId16" xr:uid="{7F5EB6BB-54CF-44D4-9A7E-43B820D52FC9}"/>
+    <hyperlink ref="D9" r:id="rId17" xr:uid="{8A381843-DB62-4AA6-A223-079DBF936DC1}"/>
+    <hyperlink ref="D10" r:id="rId18" xr:uid="{EA9D84BD-066F-4FA2-838B-E75F431BE015}"/>
+    <hyperlink ref="C11" r:id="rId19" display="manoj.pvn@heraizen.com" xr:uid="{5AD1268E-130F-49A7-B78D-449ADBD843AD}"/>
+    <hyperlink ref="C12" r:id="rId20" display="rajesh.t@heraizen.com" xr:uid="{AF0F7D47-8306-48A3-93A9-99A6183F9A7F}"/>
+    <hyperlink ref="C13" r:id="rId21" display="kalyan.k@heraizen.com" xr:uid="{B846E60B-6270-4B72-A367-AAF47167F674}"/>
+    <hyperlink ref="D11" r:id="rId22" xr:uid="{3E98E9A6-4CD0-422B-8D1B-8B46AA1F6758}"/>
+    <hyperlink ref="D12" r:id="rId23" xr:uid="{A5A2E440-80CE-4652-A96F-E54FC849E576}"/>
+    <hyperlink ref="D13" r:id="rId24" xr:uid="{F39A2176-D93A-4235-82F7-5E571E930B71}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>